<commit_message>
05.08 requirement list 수정3
</commit_message>
<xml_diff>
--- a/requirement list 1 1.xlsx
+++ b/requirement list 1 1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EE5C34C-9AA6-4F4C-B31D-F21A7720DF68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6490F648-F6D6-435D-83B2-7263808EE6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,13 +48,13 @@
     <t>대여소 검색</t>
   </si>
   <si>
-    <t>대여소 리스트에서 특정 대여소를 선택해 상세 정보 조회(대여소 이름, 대여소 위치, 사용 가능 자전거 목록 등), 대여소에 자전거가 없는 경우 예약대기 신청, 문자 알림을 통해 해당 내용 수신</t>
+    <t>대여소 리스트에서 특정 대여소를 선택해 상세 정보 조회(대여소 이름, 대여소 위치, 사용 가능 자전거 목록 등), 대여소에 자전거가 없는 경우 예약대기 신청하고 문자 알림을 통해 해당 내용 수신</t>
   </si>
   <si>
     <t>대여소 상세 정보 조회(+ 자전거 예약 대기 신청)</t>
   </si>
   <si>
-    <t>대여소에 자전거가 남아 있는 경우 즉시 대여, 문자 알림을 통해 해당 내용 수신</t>
+    <t>대여소에 자전거가 남아 있는 경우 즉시 대여하고 문자 알림을 통해 해당 내용 수신</t>
   </si>
   <si>
     <t>자전거 즉시 대여</t>
@@ -447,7 +447,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>